<commit_message>
add observed fish functionality to electrofishing data input #605
</commit_message>
<xml_diff>
--- a/bio_diversity/static/data_templates/coldbrook-electrofishing.xlsx
+++ b/bio_diversity/static/data_templates/coldbrook-electrofishing.xlsx
@@ -12,8 +12,8 @@
     <workbookView xWindow="0" yWindow="75" windowWidth="22980" windowHeight="9525"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Template" sheetId="1" r:id="rId1"/>
+    <sheet name="Sample Data" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="32">
   <si>
     <t>River</t>
   </si>
@@ -62,9 +62,6 @@
     <t>fishing minutes</t>
   </si>
   <si>
-    <t># of salmon observed/collected</t>
-  </si>
-  <si>
     <t>Settings</t>
   </si>
   <si>
@@ -77,7 +74,49 @@
     <t>Branch</t>
   </si>
   <si>
-    <t>Date (YYYY-mm-dd)</t>
+    <t>Date</t>
+  </si>
+  <si>
+    <t># of salmon collected</t>
+  </si>
+  <si>
+    <t># of salmon observed</t>
+  </si>
+  <si>
+    <t>SMA</t>
+  </si>
+  <si>
+    <t>west</t>
+  </si>
+  <si>
+    <t>fall parr collections</t>
+  </si>
+  <si>
+    <t>DC 36%, 60 Hz</t>
+  </si>
+  <si>
+    <t>Indian Man</t>
+  </si>
+  <si>
+    <t>spot check for wild salmon</t>
+  </si>
+  <si>
+    <t>AB</t>
+  </si>
+  <si>
+    <t>CD, EF, GH</t>
+  </si>
+  <si>
+    <t>at base of fall</t>
+  </si>
+  <si>
+    <t>2020-Jan-01</t>
+  </si>
+  <si>
+    <t>fished in river</t>
+  </si>
+  <si>
+    <t>saw 16 fish</t>
   </si>
 </sst>
 </file>
@@ -924,31 +963,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S6"/>
+  <dimension ref="A1:T6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.28515625" customWidth="1"/>
-    <col min="4" max="4" width="32.5703125" customWidth="1"/>
-    <col min="8" max="8" width="18.5703125" customWidth="1"/>
-    <col min="9" max="9" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.7109375" customWidth="1"/>
+    <col min="2" max="2" width="5.42578125" customWidth="1"/>
+    <col min="3" max="3" width="8.42578125" customWidth="1"/>
+    <col min="4" max="4" width="13.140625" customWidth="1"/>
+    <col min="8" max="8" width="15.140625" customWidth="1"/>
+    <col min="9" max="9" width="14.42578125" customWidth="1"/>
+    <col min="10" max="10" width="12.7109375" customWidth="1"/>
     <col min="17" max="17" width="12.5703125" customWidth="1"/>
+    <col min="18" max="18" width="17.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>1</v>
@@ -987,19 +1029,22 @@
         <v>12</v>
       </c>
       <c r="P1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="R1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="S1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="T1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="S1" s="2" t="s">
-        <v>16</v>
-      </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="5"/>
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
@@ -1019,17 +1064,19 @@
       <c r="R2" s="6"/>
       <c r="S2" s="6"/>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="5"/>
       <c r="B3" s="6"/>
       <c r="C3" s="6"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
       <c r="H3" s="7"/>
       <c r="I3" s="10"/>
       <c r="J3" s="10"/>
       <c r="K3" s="11"/>
       <c r="O3" s="8"/>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="5"/>
       <c r="B4" s="6"/>
       <c r="C4" s="6"/>
@@ -1040,7 +1087,7 @@
       <c r="K4" s="11"/>
       <c r="O4" s="8"/>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" s="5"/>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
@@ -1051,7 +1098,7 @@
       <c r="K5" s="11"/>
       <c r="O5" s="8"/>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="5"/>
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
@@ -1070,12 +1117,201 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:T3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="15.7109375" customWidth="1"/>
+    <col min="2" max="2" width="5.42578125" customWidth="1"/>
+    <col min="3" max="3" width="8.42578125" customWidth="1"/>
+    <col min="4" max="4" width="13.140625" customWidth="1"/>
+    <col min="8" max="8" width="15.140625" customWidth="1"/>
+    <col min="9" max="9" width="14.42578125" customWidth="1"/>
+    <col min="10" max="10" width="12.7109375" customWidth="1"/>
+    <col min="18" max="18" width="17.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="O1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="T1" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="F2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G2" t="s">
+        <v>27</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="I2" s="10">
+        <v>0.5625</v>
+      </c>
+      <c r="J2" s="10">
+        <v>0.64583333333333337</v>
+      </c>
+      <c r="K2" s="11">
+        <v>13.6</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
+      <c r="M2">
+        <v>5000</v>
+      </c>
+      <c r="N2">
+        <v>5000</v>
+      </c>
+      <c r="O2" s="8">
+        <f t="shared" ref="O2:O3" si="0">N2/60</f>
+        <v>83.333333333333329</v>
+      </c>
+      <c r="P2">
+        <v>17</v>
+      </c>
+      <c r="R2" t="s">
+        <v>23</v>
+      </c>
+      <c r="S2">
+        <v>543</v>
+      </c>
+      <c r="T2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F3" t="s">
+        <v>26</v>
+      </c>
+      <c r="G3" t="s">
+        <v>27</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="I3" s="10">
+        <v>0.6875</v>
+      </c>
+      <c r="J3" s="9">
+        <v>0.70763888888888893</v>
+      </c>
+      <c r="K3" s="11">
+        <v>13.5</v>
+      </c>
+      <c r="L3">
+        <v>5000</v>
+      </c>
+      <c r="M3">
+        <v>5422</v>
+      </c>
+      <c r="N3">
+        <v>422</v>
+      </c>
+      <c r="O3" s="8">
+        <f t="shared" si="0"/>
+        <v>7.0333333333333332</v>
+      </c>
+      <c r="Q3">
+        <v>16</v>
+      </c>
+      <c r="R3" t="s">
+        <v>23</v>
+      </c>
+      <c r="S3">
+        <v>543</v>
+      </c>
+      <c r="T3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
clean up data templates
</commit_message>
<xml_diff>
--- a/bio_diversity/static/data_templates/coldbrook-electrofishing.xlsx
+++ b/bio_diversity/static/data_templates/coldbrook-electrofishing.xlsx
@@ -12,9 +12,9 @@
     <workbookView xWindow="0" yWindow="75" windowWidth="22980" windowHeight="9525"/>
   </bookViews>
   <sheets>
-    <sheet name="Template" sheetId="1" r:id="rId1"/>
-    <sheet name="Sample Data" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Template" sheetId="3" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId2"/>
+    <sheet name="Sample Data" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
 </workbook>
@@ -963,24 +963,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T6"/>
+  <dimension ref="A1:T1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="15.7109375" customWidth="1"/>
-    <col min="2" max="2" width="5.42578125" customWidth="1"/>
-    <col min="3" max="3" width="8.42578125" customWidth="1"/>
-    <col min="4" max="4" width="13.140625" customWidth="1"/>
-    <col min="8" max="8" width="15.140625" customWidth="1"/>
-    <col min="9" max="9" width="14.42578125" customWidth="1"/>
-    <col min="10" max="10" width="12.7109375" customWidth="1"/>
-    <col min="17" max="17" width="12.5703125" customWidth="1"/>
-    <col min="18" max="18" width="17.85546875" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -1043,71 +1032,6 @@
       <c r="T1" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A2" s="5"/>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="10"/>
-      <c r="J2" s="10"/>
-      <c r="K2" s="8"/>
-      <c r="L2" s="6"/>
-      <c r="M2" s="6"/>
-      <c r="N2" s="6"/>
-      <c r="O2" s="8"/>
-      <c r="P2" s="6"/>
-      <c r="Q2" s="6"/>
-      <c r="R2" s="6"/>
-      <c r="S2" s="6"/>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A3" s="5"/>
-      <c r="B3" s="6"/>
-      <c r="C3" s="6"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7"/>
-      <c r="I3" s="10"/>
-      <c r="J3" s="10"/>
-      <c r="K3" s="11"/>
-      <c r="O3" s="8"/>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A4" s="5"/>
-      <c r="B4" s="6"/>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
-      <c r="H4" s="7"/>
-      <c r="I4" s="10"/>
-      <c r="J4" s="10"/>
-      <c r="K4" s="11"/>
-      <c r="O4" s="8"/>
-    </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A5" s="5"/>
-      <c r="B5" s="6"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="H5" s="7"/>
-      <c r="I5" s="9"/>
-      <c r="J5" s="9"/>
-      <c r="K5" s="11"/>
-      <c r="O5" s="8"/>
-    </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A6" s="5"/>
-      <c r="B6" s="6"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="H6" s="7"/>
-      <c r="I6" s="9"/>
-      <c r="J6" s="9"/>
-      <c r="K6" s="11"/>
-      <c r="O6" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1116,6 +1040,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T3"/>
   <sheetViews>
@@ -1315,17 +1252,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
add spawning templates and clean up templates
</commit_message>
<xml_diff>
--- a/bio_diversity/static/data_templates/coldbrook-electrofishing.xlsx
+++ b/bio_diversity/static/data_templates/coldbrook-electrofishing.xlsx
@@ -13,8 +13,7 @@
   </bookViews>
   <sheets>
     <sheet name="Template" sheetId="3" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="4" r:id="rId2"/>
-    <sheet name="Sample Data" sheetId="2" r:id="rId3"/>
+    <sheet name="Sample Data" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
 </workbook>
@@ -966,7 +965,7 @@
   <dimension ref="A1:T1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1040,19 +1039,6 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T3"/>
   <sheetViews>

</xml_diff>

<commit_message>
improve roobustness of data loader
</commit_message>
<xml_diff>
--- a/bio_diversity/static/data_templates/coldbrook-electrofishing.xlsx
+++ b/bio_diversity/static/data_templates/coldbrook-electrofishing.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="32">
   <si>
     <t>River</t>
   </si>
@@ -962,15 +962,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T1"/>
+  <dimension ref="A1:S1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>17</v>
       </c>
@@ -978,57 +976,54 @@
         <v>0</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D1" s="2" t="s">
         <v>1</v>
       </c>
+      <c r="D1" s="3" t="s">
+        <v>2</v>
+      </c>
       <c r="E1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="3" t="s">
         <v>3</v>
       </c>
+      <c r="F1" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="G1" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="N1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="N1" s="4" t="s">
         <v>12</v>
       </c>
+      <c r="O1" s="2" t="s">
+        <v>18</v>
+      </c>
       <c r="P1" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="Q1" s="2" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="R1" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="S1" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="T1" s="2" t="s">
         <v>15</v>
       </c>
     </row>

</xml_diff>

<commit_message>
split template dates into three columns, #638
</commit_message>
<xml_diff>
--- a/bio_diversity/static/data_templates/coldbrook-electrofishing.xlsx
+++ b/bio_diversity/static/data_templates/coldbrook-electrofishing.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="35">
   <si>
     <t>River</t>
   </si>
@@ -116,6 +116,15 @@
   </si>
   <si>
     <t>saw 16 fish</t>
+  </si>
+  <si>
+    <t>Year</t>
+  </si>
+  <si>
+    <t>Month</t>
+  </si>
+  <si>
+    <t>Day</t>
   </si>
 </sst>
 </file>
@@ -962,68 +971,76 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S1"/>
+  <dimension ref="A1:U1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>17</v>
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>32</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="P1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="R1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="S1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="T1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="U1" s="2" t="s">
         <v>15</v>
       </c>
     </row>

</xml_diff>

<commit_message>
rework group detail parser, in progress, #674
</commit_message>
<xml_diff>
--- a/bio_diversity/static/data_templates/coldbrook-electrofishing.xlsx
+++ b/bio_diversity/static/data_templates/coldbrook-electrofishing.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="75" windowWidth="22980" windowHeight="9525" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="75" windowWidth="22980" windowHeight="9525"/>
   </bookViews>
   <sheets>
     <sheet name="Template" sheetId="3" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="38">
   <si>
     <t>River</t>
   </si>
@@ -128,6 +128,12 @@
   </si>
   <si>
     <t>(WS)</t>
+  </si>
+  <si>
+    <t>Group</t>
+  </si>
+  <si>
+    <t>Bonell</t>
   </si>
 </sst>
 </file>
@@ -975,18 +981,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y1"/>
+  <dimension ref="A1:Z1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M1" sqref="M1:M1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="13" max="13" width="10.28515625" customWidth="1"/>
+    <col min="14" max="14" width="10.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>23</v>
       </c>
@@ -1024,42 +1030,45 @@
         <v>4</v>
       </c>
       <c r="M1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="N1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="R1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="S1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="T1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="T1" s="4" t="s">
+      <c r="U1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="V1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="V1" s="2" t="s">
+      <c r="W1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="W1" s="2" t="s">
+      <c r="X1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="X1" s="2" t="s">
+      <c r="Y1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="Y1" s="2" t="s">
+      <c r="Z1" s="2" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1071,10 +1080,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y12"/>
+  <dimension ref="A1:Z12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1088,13 +1097,13 @@
     <col min="8" max="8" width="15.140625" customWidth="1"/>
     <col min="9" max="9" width="14.42578125" customWidth="1"/>
     <col min="10" max="10" width="12.7109375" customWidth="1"/>
-    <col min="12" max="12" width="12.85546875" customWidth="1"/>
-    <col min="13" max="13" width="24.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="15" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="17.85546875" customWidth="1"/>
+    <col min="12" max="13" width="12.85546875" customWidth="1"/>
+    <col min="14" max="14" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="17.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>23</v>
       </c>
@@ -1132,46 +1141,49 @@
         <v>4</v>
       </c>
       <c r="M1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="N1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="R1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="S1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="T1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="T1" s="4" t="s">
+      <c r="U1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="V1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="V1" s="2" t="s">
+      <c r="W1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="W1" s="2" t="s">
+      <c r="X1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="X1" s="2" t="s">
+      <c r="Y1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="Y1" s="2" t="s">
+      <c r="Z1" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" s="11">
         <v>2020</v>
       </c>
@@ -1202,45 +1214,48 @@
       <c r="L2" t="s">
         <v>20</v>
       </c>
-      <c r="M2" s="6" t="s">
+      <c r="M2" t="s">
+        <v>37</v>
+      </c>
+      <c r="N2" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="N2" s="9">
+      <c r="O2" s="9">
         <v>0.5625</v>
       </c>
-      <c r="O2" s="9">
+      <c r="P2" s="9">
         <v>0.64583333333333337</v>
       </c>
-      <c r="P2" s="10">
+      <c r="Q2" s="10">
         <v>13.6</v>
       </c>
-      <c r="Q2">
+      <c r="R2">
         <v>0</v>
-      </c>
-      <c r="R2">
-        <v>5000</v>
       </c>
       <c r="S2">
         <v>5000</v>
       </c>
-      <c r="T2" s="7">
-        <f t="shared" ref="T2:T3" si="0">S2/60</f>
+      <c r="T2">
+        <v>5000</v>
+      </c>
+      <c r="U2" s="7">
+        <f t="shared" ref="U2:U3" si="0">T2/60</f>
         <v>83.333333333333329</v>
       </c>
-      <c r="U2">
+      <c r="V2">
         <v>17</v>
       </c>
-      <c r="W2" t="s">
+      <c r="X2" t="s">
         <v>18</v>
       </c>
-      <c r="X2">
+      <c r="Y2">
         <v>543</v>
       </c>
-      <c r="Y2" t="s">
+      <c r="Z2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" s="11">
         <v>2020</v>
       </c>
@@ -1277,69 +1292,69 @@
       <c r="L3" t="s">
         <v>20</v>
       </c>
-      <c r="M3" s="6" t="s">
+      <c r="N3" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="N3" s="9">
+      <c r="O3" s="9">
         <v>0.6875</v>
       </c>
-      <c r="O3" s="8">
+      <c r="P3" s="8">
         <v>0.70763888888888893</v>
       </c>
-      <c r="P3" s="10">
+      <c r="Q3" s="10">
         <v>13.5</v>
       </c>
-      <c r="Q3">
+      <c r="R3">
         <v>5000</v>
       </c>
-      <c r="R3">
+      <c r="S3">
         <v>5422</v>
       </c>
-      <c r="S3">
+      <c r="T3">
         <v>422</v>
       </c>
-      <c r="T3" s="7">
+      <c r="U3" s="7">
         <f t="shared" si="0"/>
         <v>7.0333333333333332</v>
       </c>
-      <c r="V3">
+      <c r="W3">
         <v>16</v>
       </c>
-      <c r="W3" t="s">
+      <c r="X3" t="s">
         <v>18</v>
       </c>
-      <c r="X3">
+      <c r="Y3">
         <v>543</v>
       </c>
-      <c r="Y3" t="s">
+      <c r="Z3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4" s="12"/>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A5" s="12"/>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6" s="12"/>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A7" s="12"/>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A8" s="12"/>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A9" s="12"/>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A10" s="12"/>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A11" s="12"/>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A12" s="12"/>
     </row>
   </sheetData>

</xml_diff>